<commit_message>
Up to Release V.1.5 Complete Code Improvement Customer DemoGraphic API and Locator Update GSM KYC Profile and KYC Profile API Automation Loan Widget API Automation Recharge History API Automation Backend Agent and Backend Supervisor Common POM Implementation Transfer to queue Data from Excel Widget API & Element locator Update
</commit_message>
<xml_diff>
--- a/Excels/MW.xlsx
+++ b/Excels/MW.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="35835" windowHeight="20280" firstSheet="12" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Authentication Policy" sheetId="18" r:id="rId13"/>
     <sheet name="Action Tagging" sheetId="19" r:id="rId14"/>
     <sheet name="State Queue Mapping" sheetId="20" r:id="rId15"/>
+    <sheet name="Transfer To Queue" sheetId="21" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'FTRTickets-Reg'!$A$1:$F$131</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1953" uniqueCount="926">
   <si>
     <t>loginAuuid</t>
   </si>
@@ -2489,457 +2490,340 @@
     <t>COM084</t>
   </si>
   <si>
-    <t>210820000136</t>
-  </si>
-  <si>
-    <t>210820000137</t>
-  </si>
-  <si>
-    <t>210820000138</t>
-  </si>
-  <si>
-    <t>210820000139</t>
-  </si>
-  <si>
-    <t>210820000140</t>
-  </si>
-  <si>
-    <t>210820000141</t>
-  </si>
-  <si>
-    <t>210820000142</t>
-  </si>
-  <si>
-    <t>210820000143</t>
-  </si>
-  <si>
-    <t>210820000144</t>
-  </si>
-  <si>
-    <t>210820000145</t>
+    <t>030920000221</t>
+  </si>
+  <si>
+    <t>030920000222</t>
+  </si>
+  <si>
+    <t>030920000223</t>
+  </si>
+  <si>
+    <t>030920000224</t>
+  </si>
+  <si>
+    <t>030920000225</t>
+  </si>
+  <si>
+    <t>030920000226</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>Langugae</t>
+  </si>
+  <si>
+    <t>CS Profile Management</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>CS SMS Management</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Customer Service Backend Agent</t>
+  </si>
+  <si>
+    <t>Swahili</t>
+  </si>
+  <si>
+    <t>Customer Service Frontend Agent</t>
+  </si>
+  <si>
+    <t>Customer Service Backend Supervisor</t>
+  </si>
+  <si>
+    <t>NFTR Issue Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ticket From State </t>
+  </si>
+  <si>
+    <t>Ticket To State</t>
+  </si>
+  <si>
+    <t>From Queue</t>
+  </si>
+  <si>
+    <t>To Queue</t>
+  </si>
+  <si>
+    <t>Available Credit Balance (For Prepaid)</t>
+  </si>
+  <si>
+    <t>Last Recharge Date (For Pre-Paid)</t>
+  </si>
+  <si>
+    <t>Frequently dialled number (at least two) – 2 last dialled number, validated on ECMS:</t>
+  </si>
+  <si>
+    <t>Last Recharge Value (For Prepaid)</t>
+  </si>
+  <si>
+    <t>National ID/Passport/Alien Number (Mandatory)</t>
+  </si>
+  <si>
+    <t>Customer Name (Mandatory)</t>
+  </si>
+  <si>
+    <t>No authentication policy statement configured</t>
+  </si>
+  <si>
+    <t>KE Action Authentication</t>
+  </si>
+  <si>
+    <t>Question10</t>
+  </si>
+  <si>
+    <t>Question9</t>
+  </si>
+  <si>
+    <t>Question8</t>
+  </si>
+  <si>
+    <t>Question7</t>
+  </si>
+  <si>
+    <t>Question6</t>
+  </si>
+  <si>
+    <t>Question5</t>
+  </si>
+  <si>
+    <t>Question4</t>
+  </si>
+  <si>
+    <t>Question3</t>
+  </si>
+  <si>
+    <t>Question2</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Minimum Question</t>
+  </si>
+  <si>
+    <t>Policy Message</t>
+  </si>
+  <si>
+    <t>Policy Name</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Option1</t>
+  </si>
+  <si>
+    <t>Option2</t>
+  </si>
+  <si>
+    <t>Option3</t>
+  </si>
+  <si>
+    <t>Option4</t>
+  </si>
+  <si>
+    <t>Option5</t>
+  </si>
+  <si>
+    <t>Category code</t>
+  </si>
+  <si>
+    <t>SIM Bar Unbar</t>
+  </si>
+  <si>
+    <t>SIM Lost</t>
+  </si>
+  <si>
+    <t>SIM Broken</t>
+  </si>
+  <si>
+    <t>Queue Name</t>
+  </si>
+  <si>
+    <t>State name1</t>
+  </si>
+  <si>
+    <t>State name2</t>
+  </si>
+  <si>
+    <t>State name3</t>
+  </si>
+  <si>
+    <t>State name4</t>
+  </si>
+  <si>
+    <t>State name5</t>
+  </si>
+  <si>
+    <t>State name6</t>
+  </si>
+  <si>
+    <t>State name7</t>
+  </si>
+  <si>
+    <t>State name8</t>
+  </si>
+  <si>
+    <t>State name9</t>
+  </si>
+  <si>
+    <t>State name10</t>
+  </si>
+  <si>
+    <t>Corporate with CRM</t>
+  </si>
+  <si>
+    <t>Issue Field 7 - Label</t>
+  </si>
+  <si>
+    <t>Field 7 Type</t>
+  </si>
+  <si>
+    <t>Workgroup 2</t>
+  </si>
+  <si>
+    <t>SLA2 ( Hrs : Mins)</t>
+  </si>
+  <si>
+    <t>Workgroup 3</t>
+  </si>
+  <si>
+    <t>SLA3 ( Hrs : Mins)</t>
+  </si>
+  <si>
+    <t>Workgroup 4</t>
+  </si>
+  <si>
+    <t>SLA4 ( Hrs : Mins)</t>
+  </si>
+  <si>
+    <t>Total Committed SLA</t>
+  </si>
+  <si>
+    <t>QWlydGVsIzMyMQ</t>
+  </si>
+  <si>
+    <t>U2VwdEAxMjMk</t>
+  </si>
+  <si>
+    <t>S3l1Y2hheWllQDEyMw</t>
+  </si>
+  <si>
+    <t>Ticket Field 1 - Label</t>
+  </si>
+  <si>
+    <t>Ticket 1 Type</t>
+  </si>
+  <si>
+    <t>Ticket Field 2 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 3 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 4 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 5 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 6 - Label</t>
+  </si>
+  <si>
+    <t>Ticket Field 7 - Label</t>
+  </si>
+  <si>
+    <t>910820000143</t>
   </si>
   <si>
     <t>210820000146</t>
   </si>
   <si>
-    <t>210820000147</t>
-  </si>
-  <si>
-    <t>210820000148</t>
-  </si>
-  <si>
-    <t>210820000149</t>
-  </si>
-  <si>
-    <t>210820000150</t>
-  </si>
-  <si>
-    <t>210820000151</t>
-  </si>
-  <si>
-    <t>210820000152</t>
-  </si>
-  <si>
-    <t>210820000153</t>
-  </si>
-  <si>
-    <t>210820000154</t>
-  </si>
-  <si>
-    <t>210820000155</t>
-  </si>
-  <si>
-    <t>210820000156</t>
-  </si>
-  <si>
-    <t>210820000157</t>
-  </si>
-  <si>
-    <t>210820000158</t>
-  </si>
-  <si>
-    <t>210820000160</t>
-  </si>
-  <si>
-    <t>210820000161</t>
-  </si>
-  <si>
-    <t>210820000162</t>
-  </si>
-  <si>
-    <t>210820000163</t>
-  </si>
-  <si>
-    <t>210820000164</t>
-  </si>
-  <si>
-    <t>210820000165</t>
-  </si>
-  <si>
-    <t>210820000166</t>
-  </si>
-  <si>
-    <t>210820000167</t>
-  </si>
-  <si>
-    <t>210820000168</t>
-  </si>
-  <si>
-    <t>210820000169</t>
-  </si>
-  <si>
-    <t>210820000170</t>
-  </si>
-  <si>
-    <t>210820000171</t>
-  </si>
-  <si>
-    <t>210820000172</t>
-  </si>
-  <si>
-    <t>210820000173</t>
-  </si>
-  <si>
-    <t>210820000174</t>
-  </si>
-  <si>
-    <t>210820000175</t>
-  </si>
-  <si>
-    <t>210820000176</t>
-  </si>
-  <si>
-    <t>210820000177</t>
-  </si>
-  <si>
-    <t>210820000178</t>
-  </si>
-  <si>
-    <t>210820000179</t>
-  </si>
-  <si>
-    <t>210820000180</t>
-  </si>
-  <si>
-    <t>210820000181</t>
-  </si>
-  <si>
-    <t>210820000182</t>
-  </si>
-  <si>
-    <t>210820000183</t>
-  </si>
-  <si>
-    <t>210820000184</t>
-  </si>
-  <si>
-    <t>210820000185</t>
-  </si>
-  <si>
-    <t>210820000186</t>
-  </si>
-  <si>
-    <t>210820000187</t>
-  </si>
-  <si>
-    <t>210820000188</t>
-  </si>
-  <si>
-    <t>210820000189</t>
-  </si>
-  <si>
-    <t>210820000190</t>
-  </si>
-  <si>
-    <t>210820000191</t>
-  </si>
-  <si>
-    <t>210820000192</t>
-  </si>
-  <si>
-    <t>210820000193</t>
-  </si>
-  <si>
-    <t>210820000194</t>
-  </si>
-  <si>
-    <t>210820000195</t>
-  </si>
-  <si>
-    <t>210820000196</t>
-  </si>
-  <si>
-    <t>210820000197</t>
-  </si>
-  <si>
-    <t>210820000198</t>
-  </si>
-  <si>
-    <t>210820000199</t>
-  </si>
-  <si>
-    <t>210820000200</t>
-  </si>
-  <si>
-    <t>210820000201</t>
-  </si>
-  <si>
-    <t>210820000202</t>
-  </si>
-  <si>
-    <t>210820000203</t>
-  </si>
-  <si>
-    <t>210820000204</t>
-  </si>
-  <si>
-    <t>210820000205</t>
-  </si>
-  <si>
-    <t>210820000206</t>
-  </si>
-  <si>
-    <t>210820000207</t>
-  </si>
-  <si>
-    <t>210820000208</t>
-  </si>
-  <si>
-    <t>210820000209</t>
-  </si>
-  <si>
-    <t>210820000210</t>
-  </si>
-  <si>
-    <t>210820000211</t>
-  </si>
-  <si>
-    <t>Rm9yZ290QDEyMw</t>
-  </si>
-  <si>
-    <t>U2FmZUAxMjM</t>
-  </si>
-  <si>
-    <t>030920000221</t>
-  </si>
-  <si>
-    <t>030920000222</t>
-  </si>
-  <si>
-    <t>030920000223</t>
-  </si>
-  <si>
-    <t>030920000224</t>
-  </si>
-  <si>
-    <t>030920000225</t>
-  </si>
-  <si>
-    <t>030920000226</t>
-  </si>
-  <si>
-    <t>Roles</t>
-  </si>
-  <si>
-    <t>Langugae</t>
-  </si>
-  <si>
-    <t>CS Profile Management</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>CS SMS Management</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>Customer Service Backend Agent</t>
-  </si>
-  <si>
-    <t>Swahili</t>
-  </si>
-  <si>
-    <t>Customer Service Frontend Agent</t>
-  </si>
-  <si>
-    <t>Customer Service Backend Supervisor</t>
-  </si>
-  <si>
-    <t>NFTR Issue Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ticket From State </t>
-  </si>
-  <si>
-    <t>Ticket To State</t>
-  </si>
-  <si>
-    <t>From Queue</t>
-  </si>
-  <si>
-    <t>To Queue</t>
-  </si>
-  <si>
-    <t>Available Credit Balance (For Prepaid)</t>
-  </si>
-  <si>
-    <t>Last Recharge Date (For Pre-Paid)</t>
-  </si>
-  <si>
-    <t>Frequently dialled number (at least two) – 2 last dialled number, validated on ECMS:</t>
-  </si>
-  <si>
-    <t>Last Recharge Value (For Prepaid)</t>
-  </si>
-  <si>
-    <t>National ID/Passport/Alien Number (Mandatory)</t>
-  </si>
-  <si>
-    <t>Customer Name (Mandatory)</t>
-  </si>
-  <si>
-    <t>No authentication policy statement configured</t>
-  </si>
-  <si>
-    <t>KE Action Authentication</t>
-  </si>
-  <si>
-    <t>Question10</t>
-  </si>
-  <si>
-    <t>Question9</t>
-  </si>
-  <si>
-    <t>Question8</t>
-  </si>
-  <si>
-    <t>Question7</t>
-  </si>
-  <si>
-    <t>Question6</t>
-  </si>
-  <si>
-    <t>Question5</t>
-  </si>
-  <si>
-    <t>Question4</t>
-  </si>
-  <si>
-    <t>Question3</t>
-  </si>
-  <si>
-    <t>Question2</t>
-  </si>
-  <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Minimum Question</t>
-  </si>
-  <si>
-    <t>Policy Message</t>
-  </si>
-  <si>
-    <t>Policy Name</t>
-  </si>
-  <si>
-    <t>Action</t>
-  </si>
-  <si>
-    <t>Option1</t>
-  </si>
-  <si>
-    <t>Option2</t>
-  </si>
-  <si>
-    <t>Option3</t>
-  </si>
-  <si>
-    <t>Option4</t>
-  </si>
-  <si>
-    <t>Option5</t>
-  </si>
-  <si>
-    <t>Category code</t>
-  </si>
-  <si>
-    <t>SIM Bar Unbar</t>
-  </si>
-  <si>
-    <t>SIM Lost</t>
-  </si>
-  <si>
-    <t>SIM Broken</t>
-  </si>
-  <si>
-    <t>Queue Name</t>
-  </si>
-  <si>
-    <t>State name1</t>
-  </si>
-  <si>
-    <t>State name2</t>
-  </si>
-  <si>
-    <t>State name3</t>
-  </si>
-  <si>
-    <t>State name4</t>
-  </si>
-  <si>
-    <t>State name5</t>
-  </si>
-  <si>
-    <t>State name6</t>
-  </si>
-  <si>
-    <t>State name7</t>
-  </si>
-  <si>
-    <t>State name8</t>
-  </si>
-  <si>
-    <t>State name9</t>
-  </si>
-  <si>
-    <t>State name10</t>
-  </si>
-  <si>
-    <t>Corporate with CRM</t>
-  </si>
-  <si>
-    <t>Issue Field 7 - Label</t>
-  </si>
-  <si>
-    <t>Field 7 Type</t>
-  </si>
-  <si>
-    <t>Workgroup 2</t>
-  </si>
-  <si>
-    <t>SLA2 ( Hrs : Mins)</t>
-  </si>
-  <si>
-    <t>Workgroup 3</t>
-  </si>
-  <si>
-    <t>SLA3 ( Hrs : Mins)</t>
-  </si>
-  <si>
-    <t>Workgroup 4</t>
-  </si>
-  <si>
-    <t>SLA4 ( Hrs : Mins)</t>
-  </si>
-  <si>
-    <t>Total Committed SLA</t>
-  </si>
-  <si>
-    <t>U2VwdEAxMjMk</t>
+    <t>Outbound</t>
+  </si>
+  <si>
+    <t>Loan Services</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Loan Amount (Ksh)</t>
+  </si>
+  <si>
+    <t>Credited On</t>
+  </si>
+  <si>
+    <t>Current Outstanding</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Loan Details</t>
+  </si>
+  <si>
+    <t>Total Loan Eligibility</t>
+  </si>
+  <si>
+    <t>Number of Loan Taken</t>
+  </si>
+  <si>
+    <t>Total Loan Amount</t>
+  </si>
+  <si>
+    <t>Total Loan Paid</t>
+  </si>
+  <si>
+    <t>Total Current Outstanding</t>
+  </si>
+  <si>
+    <t>Loan History</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Amount Credited</t>
+  </si>
+  <si>
+    <t>Service Charge</t>
+  </si>
+  <si>
+    <t>Recovered</t>
+  </si>
+  <si>
+    <t>Loan Channel</t>
+  </si>
+  <si>
+    <t>Loan Type</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Loan Recoveries</t>
+  </si>
+  <si>
+    <t>Transaction ID</t>
+  </si>
+  <si>
+    <t>Amount Recovered</t>
+  </si>
+  <si>
+    <t>Recovery Method</t>
+  </si>
+  <si>
+    <t>Date Recovered</t>
   </si>
 </sst>
 </file>
@@ -3012,6 +2896,7 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -3148,7 +3033,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3197,6 +3082,8 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3257,6 +3144,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="1800225"/>
+          <a:ext cx="304800" cy="301625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{954E16FB-6A94-A343-90CA-E894AD77BEF0}"/>
@@ -3591,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3656,7 +3591,7 @@
         <v>2390495</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>964</v>
+        <v>888</v>
       </c>
       <c r="C2" t="s">
         <v>67</v>
@@ -3703,7 +3638,7 @@
         <v>2388192</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="C3" t="s">
         <v>66</v>
@@ -3714,7 +3649,7 @@
         <v>2390495</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>964</v>
+        <v>888</v>
       </c>
       <c r="C4" t="s">
         <v>175</v>
@@ -3837,39 +3772,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>897</v>
+        <v>820</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>898</v>
+        <v>821</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
-        <v>899</v>
+        <v>822</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>900</v>
+        <v>823</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>901</v>
+        <v>824</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>902</v>
+        <v>825</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
-        <v>903</v>
+        <v>826</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>904</v>
+        <v>827</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
-        <v>905</v>
+        <v>828</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3879,7 +3814,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>906</v>
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -3891,8 +3826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3905,19 +3840,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>907</v>
+        <v>830</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>908</v>
+        <v>831</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>909</v>
+        <v>832</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>910</v>
+        <v>833</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>911</v>
+        <v>834</v>
       </c>
     </row>
   </sheetData>
@@ -3952,72 +3887,72 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>932</v>
+        <v>855</v>
       </c>
       <c r="B1" t="s">
-        <v>931</v>
+        <v>854</v>
       </c>
       <c r="C1" t="s">
-        <v>930</v>
+        <v>853</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>929</v>
+        <v>852</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>928</v>
+        <v>851</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>927</v>
+        <v>850</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>926</v>
+        <v>849</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>925</v>
+        <v>848</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>924</v>
+        <v>847</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>923</v>
+        <v>846</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>922</v>
+        <v>845</v>
       </c>
       <c r="L1" s="30" t="s">
-        <v>921</v>
+        <v>844</v>
       </c>
       <c r="M1" s="30" t="s">
-        <v>920</v>
+        <v>843</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>919</v>
+        <v>842</v>
       </c>
       <c r="B2" t="s">
-        <v>918</v>
+        <v>841</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>917</v>
+        <v>840</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>916</v>
+        <v>839</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>915</v>
+        <v>838</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>914</v>
+        <v>837</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>913</v>
+        <v>836</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>912</v>
+        <v>835</v>
       </c>
     </row>
   </sheetData>
@@ -4042,36 +3977,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>933</v>
+        <v>856</v>
       </c>
       <c r="B1" t="s">
-        <v>934</v>
+        <v>857</v>
       </c>
       <c r="C1" t="s">
-        <v>935</v>
+        <v>858</v>
       </c>
       <c r="D1" t="s">
-        <v>936</v>
+        <v>859</v>
       </c>
       <c r="E1" t="s">
-        <v>937</v>
+        <v>860</v>
       </c>
       <c r="F1" t="s">
-        <v>938</v>
+        <v>861</v>
       </c>
       <c r="G1" t="s">
-        <v>939</v>
+        <v>862</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>940</v>
+        <v>863</v>
       </c>
       <c r="B2" t="s">
-        <v>941</v>
+        <v>864</v>
       </c>
       <c r="C2" t="s">
-        <v>942</v>
+        <v>865</v>
       </c>
     </row>
   </sheetData>
@@ -4099,42 +4034,42 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>943</v>
+        <v>866</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>944</v>
+        <v>867</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>945</v>
+        <v>868</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>946</v>
+        <v>869</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>947</v>
+        <v>870</v>
       </c>
       <c r="F1" s="31" t="s">
-        <v>948</v>
+        <v>871</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>949</v>
+        <v>872</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>950</v>
+        <v>873</v>
       </c>
       <c r="I1" s="31" t="s">
-        <v>951</v>
+        <v>874</v>
       </c>
       <c r="J1" s="31" t="s">
-        <v>952</v>
+        <v>875</v>
       </c>
       <c r="K1" s="31" t="s">
-        <v>953</v>
+        <v>876</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>954</v>
+        <v>877</v>
       </c>
       <c r="B2" s="31" t="s">
         <v>57</v>
@@ -4194,6 +4129,58 @@
       <c r="I4" s="31"/>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.125" customWidth="1"/>
+    <col min="2" max="2" width="24.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>833</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>877</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4256,10 +4243,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4490,6 +4477,100 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>901</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>902</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>903</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>904</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>905</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>906</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>907</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>908</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>909</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>911</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>912</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>913</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>914</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>915</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>916</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>917</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>921</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4499,10 +4580,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL78"/>
+  <dimension ref="A1:BG78"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AH76" sqref="AH76"/>
+    <sheetView topLeftCell="AQ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BG9" sqref="BG9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4532,7 +4613,7 @@
     <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>15</v>
       </c>
@@ -4603,52 +4684,115 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>955</v>
+        <v>878</v>
       </c>
       <c r="Y1" t="s">
-        <v>956</v>
+        <v>879</v>
       </c>
       <c r="Z1" t="s">
         <v>22</v>
       </c>
       <c r="AA1" t="s">
+        <v>890</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>891</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>892</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>893</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>894</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>895</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>896</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>897</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>879</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AW1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="36" t="s">
-        <v>957</v>
-      </c>
-      <c r="AD1" s="36" t="s">
-        <v>958</v>
-      </c>
-      <c r="AE1" s="36" t="s">
-        <v>959</v>
-      </c>
-      <c r="AF1" s="36" t="s">
-        <v>960</v>
-      </c>
-      <c r="AG1" s="36" t="s">
-        <v>961</v>
-      </c>
-      <c r="AH1" s="36" t="s">
-        <v>962</v>
-      </c>
-      <c r="AI1" s="37" t="s">
-        <v>963</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AX1" s="36" t="s">
+        <v>880</v>
+      </c>
+      <c r="AY1" s="36" t="s">
+        <v>881</v>
+      </c>
+      <c r="AZ1" s="36" t="s">
+        <v>882</v>
+      </c>
+      <c r="BA1" s="36" t="s">
+        <v>883</v>
+      </c>
+      <c r="BB1" s="36" t="s">
+        <v>884</v>
+      </c>
+      <c r="BC1" s="36" t="s">
+        <v>885</v>
+      </c>
+      <c r="BD1" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="BE1" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="BF1" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BG1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>130</v>
       </c>
@@ -4712,27 +4856,24 @@
       <c r="U2" s="19"/>
       <c r="V2" s="19"/>
       <c r="W2" s="19"/>
-      <c r="AA2" s="19" t="s">
+      <c r="AV2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI2">
-        <f>SUM(AB2,AD2,AF2,AH2)</f>
-        <v>24</v>
-      </c>
-      <c r="AJ2" s="19" t="s">
+      <c r="AW2" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD2">
+        <f>SUM(AW2,AY2,BA2,BC2)</f>
+        <v>24</v>
+      </c>
+      <c r="BE2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK2" s="19" t="s">
+      <c r="BF2" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL2" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>130</v>
       </c>
@@ -4766,27 +4907,24 @@
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
       <c r="W3" s="21"/>
-      <c r="AA3" s="21" t="s">
+      <c r="AV3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB3" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI3">
-        <f t="shared" ref="AI3:AI66" si="0">SUM(AB3,AD3,AF3,AH3)</f>
-        <v>24</v>
-      </c>
-      <c r="AJ3" s="21" t="s">
+      <c r="AW3" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD3">
+        <f t="shared" ref="BD3:BD66" si="0">SUM(AW3,AY3,BA3,BC3)</f>
+        <v>24</v>
+      </c>
+      <c r="BE3" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK3" s="21" t="s">
+      <c r="BF3" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL3" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>130</v>
       </c>
@@ -4856,27 +4994,24 @@
       <c r="W4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AA4" s="19" t="s">
+      <c r="AV4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB4" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI4">
+      <c r="AW4" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ4" s="19" t="s">
+      <c r="BE4" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK4" s="19" t="s">
+      <c r="BF4" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL4" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>130</v>
       </c>
@@ -4910,27 +5045,24 @@
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
       <c r="W5" s="21"/>
-      <c r="AA5" s="21" t="s">
+      <c r="AV5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB5" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI5">
+      <c r="AW5" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD5">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ5" s="21" t="s">
+      <c r="BE5" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK5" s="21" t="s">
+      <c r="BF5" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL5" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>130</v>
       </c>
@@ -4994,24 +5126,25 @@
       <c r="U6" s="22"/>
       <c r="V6" s="22"/>
       <c r="W6" s="19"/>
-      <c r="AA6" s="19" t="s">
+      <c r="AV6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB6" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI6">
+      <c r="AW6" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD6">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ6" s="19" t="s">
+      <c r="BE6" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK6" s="19" t="s">
+      <c r="BF6" s="19" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG6" s="38"/>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>130</v>
       </c>
@@ -5081,27 +5214,24 @@
       <c r="W7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AA7" s="21" t="s">
+      <c r="AV7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB7" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI7">
+      <c r="AW7" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ7" s="21" t="s">
+      <c r="BE7" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK7" s="21" t="s">
+      <c r="BF7" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL7" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>130</v>
       </c>
@@ -5165,27 +5295,24 @@
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
       <c r="W8" s="19"/>
-      <c r="AA8" s="19" t="s">
+      <c r="AV8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB8" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI8">
+      <c r="AW8" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD8">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ8" s="19" t="s">
+      <c r="BE8" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK8" s="19" t="s">
+      <c r="BF8" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL8" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>130</v>
       </c>
@@ -5219,27 +5346,24 @@
       <c r="U9" s="21"/>
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
-      <c r="AA9" s="21" t="s">
+      <c r="AV9" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB9" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI9">
+      <c r="AW9" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD9">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ9" s="21" t="s">
+      <c r="BE9" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK9" s="21" t="s">
+      <c r="BF9" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL9" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>130</v>
       </c>
@@ -5273,27 +5397,27 @@
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
       <c r="W10" s="19"/>
-      <c r="AA10" s="19" t="s">
+      <c r="AV10" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB10" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI10">
+      <c r="AW10" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ10" s="19" t="s">
+      <c r="BE10" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK10" s="19" t="s">
+      <c r="BF10" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL10" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG10" s="38" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>130</v>
       </c>
@@ -5327,27 +5451,27 @@
       <c r="U11" s="21"/>
       <c r="V11" s="21"/>
       <c r="W11" s="21"/>
-      <c r="AA11" s="21" t="s">
+      <c r="AV11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB11" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI11">
+      <c r="AW11" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD11">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ11" s="21" t="s">
+      <c r="BE11" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK11" s="21" t="s">
+      <c r="BF11" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL11" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG11" s="38" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>130</v>
       </c>
@@ -5381,27 +5505,24 @@
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
       <c r="W12" s="19"/>
-      <c r="AA12" s="19" t="s">
+      <c r="AV12" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB12" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI12">
+      <c r="AW12" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD12">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ12" s="19" t="s">
+      <c r="BE12" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK12" s="19" t="s">
+      <c r="BF12" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL12" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>130</v>
       </c>
@@ -5435,27 +5556,24 @@
       <c r="U13" s="21"/>
       <c r="V13" s="21"/>
       <c r="W13" s="21"/>
-      <c r="AA13" s="21" t="s">
+      <c r="AV13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB13" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI13">
+      <c r="AW13" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD13">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ13" s="21" t="s">
+      <c r="BE13" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK13" s="21" t="s">
+      <c r="BF13" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL13" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>130</v>
       </c>
@@ -5489,27 +5607,24 @@
       <c r="U14" s="19"/>
       <c r="V14" s="19"/>
       <c r="W14" s="19"/>
-      <c r="AA14" s="19" t="s">
+      <c r="AV14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB14" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI14">
+      <c r="AW14" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD14">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ14" s="19" t="s">
+      <c r="BE14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK14" s="19" t="s">
+      <c r="BF14" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL14" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>130</v>
       </c>
@@ -5543,27 +5658,24 @@
       <c r="U15" s="21"/>
       <c r="V15" s="21"/>
       <c r="W15" s="21"/>
-      <c r="AA15" s="21" t="s">
+      <c r="AV15" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB15" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI15">
+      <c r="AW15" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD15">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ15" s="21" t="s">
+      <c r="BE15" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK15" s="21" t="s">
+      <c r="BF15" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL15" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>130</v>
       </c>
@@ -5597,27 +5709,24 @@
       <c r="U16" s="19"/>
       <c r="V16" s="19"/>
       <c r="W16" s="19"/>
-      <c r="AA16" s="19" t="s">
+      <c r="AV16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB16" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI16">
+      <c r="AW16" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD16">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ16" s="19" t="s">
+      <c r="BE16" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK16" s="19" t="s">
+      <c r="BF16" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL16" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>130</v>
       </c>
@@ -5651,27 +5760,24 @@
       <c r="U17" s="21"/>
       <c r="V17" s="21"/>
       <c r="W17" s="21"/>
-      <c r="AA17" s="21" t="s">
+      <c r="AV17" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB17" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI17">
+      <c r="AW17" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD17">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ17" s="21" t="s">
+      <c r="BE17" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK17" s="21" t="s">
+      <c r="BF17" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL17" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>130</v>
       </c>
@@ -5705,27 +5811,24 @@
       <c r="U18" s="19"/>
       <c r="V18" s="19"/>
       <c r="W18" s="19"/>
-      <c r="AA18" s="19" t="s">
+      <c r="AV18" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB18" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI18">
+      <c r="AW18" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD18">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ18" s="19" t="s">
+      <c r="BE18" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK18" s="19" t="s">
+      <c r="BF18" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL18" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>631</v>
       </c>
@@ -5759,27 +5862,24 @@
       <c r="U19" s="21"/>
       <c r="V19" s="21"/>
       <c r="W19" s="21"/>
-      <c r="AA19" s="21" t="s">
+      <c r="AV19" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB19" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI19">
+      <c r="AW19" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD19">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ19" s="21" t="s">
+      <c r="BE19" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK19" s="21" t="s">
+      <c r="BF19" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL19" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>631</v>
       </c>
@@ -5813,27 +5913,24 @@
       <c r="U20" s="19"/>
       <c r="V20" s="19"/>
       <c r="W20" s="19"/>
-      <c r="AA20" s="19" t="s">
+      <c r="AV20" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB20" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI20">
+      <c r="AW20" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD20">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ20" s="19" t="s">
+      <c r="BE20" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK20" s="19" t="s">
+      <c r="BF20" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL20" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>631</v>
       </c>
@@ -5867,27 +5964,24 @@
       <c r="U21" s="21"/>
       <c r="V21" s="21"/>
       <c r="W21" s="21"/>
-      <c r="AA21" s="21" t="s">
+      <c r="AV21" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB21" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI21">
+      <c r="AW21" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD21">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ21" s="21" t="s">
+      <c r="BE21" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK21" s="21" t="s">
+      <c r="BF21" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL21" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>631</v>
       </c>
@@ -5921,27 +6015,24 @@
       <c r="U22" s="19"/>
       <c r="V22" s="19"/>
       <c r="W22" s="19"/>
-      <c r="AA22" s="19" t="s">
+      <c r="AV22" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB22" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI22">
+      <c r="AW22" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD22">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ22" s="19" t="s">
+      <c r="BE22" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK22" s="19" t="s">
+      <c r="BF22" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL22" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>631</v>
       </c>
@@ -5975,27 +6066,24 @@
       <c r="U23" s="21"/>
       <c r="V23" s="21"/>
       <c r="W23" s="21"/>
-      <c r="AA23" s="21" t="s">
+      <c r="AV23" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB23" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI23">
+      <c r="AW23" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD23">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ23" s="21" t="s">
+      <c r="BE23" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK23" s="21" t="s">
+      <c r="BF23" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL23" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>631</v>
       </c>
@@ -6029,27 +6117,24 @@
       <c r="U24" s="19"/>
       <c r="V24" s="19"/>
       <c r="W24" s="19"/>
-      <c r="AA24" s="19" t="s">
+      <c r="AV24" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB24" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI24">
+      <c r="AW24" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD24">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ24" s="19" t="s">
+      <c r="BE24" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK24" s="19" t="s">
+      <c r="BF24" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL24" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>631</v>
       </c>
@@ -6083,27 +6168,24 @@
       <c r="U25" s="21"/>
       <c r="V25" s="21"/>
       <c r="W25" s="21"/>
-      <c r="AA25" s="21" t="s">
+      <c r="AV25" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB25" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI25">
+      <c r="AW25" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ25" s="21" t="s">
+      <c r="BE25" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK25" s="21" t="s">
+      <c r="BF25" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL25" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>631</v>
       </c>
@@ -6137,24 +6219,24 @@
       <c r="U26" s="19"/>
       <c r="V26" s="19"/>
       <c r="W26" s="19"/>
-      <c r="AA26" s="19" t="s">
+      <c r="AV26" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB26" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI26">
+      <c r="AW26" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD26">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ26" s="19" t="s">
+      <c r="BE26" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK26" s="19" t="s">
+      <c r="BF26" s="19" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>631</v>
       </c>
@@ -6188,27 +6270,24 @@
       <c r="U27" s="21"/>
       <c r="V27" s="21"/>
       <c r="W27" s="21"/>
-      <c r="AA27" s="21" t="s">
+      <c r="AV27" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB27" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI27">
+      <c r="AW27" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD27">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ27" s="21" t="s">
+      <c r="BE27" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK27" s="21" t="s">
+      <c r="BF27" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL27" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>631</v>
       </c>
@@ -6242,27 +6321,24 @@
       <c r="U28" s="19"/>
       <c r="V28" s="19"/>
       <c r="W28" s="19"/>
-      <c r="AA28" s="19" t="s">
+      <c r="AV28" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB28" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI28">
+      <c r="AW28" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD28">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ28" s="19" t="s">
+      <c r="BE28" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK28" s="19" t="s">
+      <c r="BF28" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL28" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
         <v>631</v>
       </c>
@@ -6296,27 +6372,24 @@
       <c r="U29" s="21"/>
       <c r="V29" s="21"/>
       <c r="W29" s="21"/>
-      <c r="AA29" s="21" t="s">
+      <c r="AV29" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB29" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI29">
+      <c r="AW29" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD29">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ29" s="21" t="s">
+      <c r="BE29" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK29" s="21" t="s">
+      <c r="BF29" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL29" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>631</v>
       </c>
@@ -6350,27 +6423,24 @@
       <c r="U30" s="19"/>
       <c r="V30" s="19"/>
       <c r="W30" s="19"/>
-      <c r="AA30" s="19" t="s">
+      <c r="AV30" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB30" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI30">
+      <c r="AW30" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD30">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ30" s="19" t="s">
+      <c r="BE30" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK30" s="19" t="s">
+      <c r="BF30" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL30" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
         <v>631</v>
       </c>
@@ -6422,27 +6492,24 @@
       <c r="U31" s="21"/>
       <c r="V31" s="21"/>
       <c r="W31" s="21"/>
-      <c r="AA31" s="21" t="s">
+      <c r="AV31" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB31" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI31">
+      <c r="AW31" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD31">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ31" s="21" t="s">
+      <c r="BE31" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK31" s="21" t="s">
+      <c r="BF31" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL31" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>631</v>
       </c>
@@ -6476,27 +6543,24 @@
       <c r="U32" s="19"/>
       <c r="V32" s="19"/>
       <c r="W32" s="19"/>
-      <c r="AA32" s="19" t="s">
+      <c r="AV32" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB32" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI32">
+      <c r="AW32" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD32">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ32" s="19" t="s">
+      <c r="BE32" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK32" s="19" t="s">
+      <c r="BF32" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL32" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>631</v>
       </c>
@@ -6530,27 +6594,24 @@
       <c r="U33" s="21"/>
       <c r="V33" s="21"/>
       <c r="W33" s="21"/>
-      <c r="AA33" s="21" t="s">
+      <c r="AV33" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB33" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI33">
+      <c r="AW33" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD33">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ33" s="21" t="s">
+      <c r="BE33" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK33" s="21" t="s">
+      <c r="BF33" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL33" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>631</v>
       </c>
@@ -6608,27 +6669,24 @@
       <c r="U34" s="19"/>
       <c r="V34" s="19"/>
       <c r="W34" s="19"/>
-      <c r="AA34" s="19" t="s">
+      <c r="AV34" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB34" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI34">
+      <c r="AW34" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD34">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ34" s="19" t="s">
+      <c r="BE34" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK34" s="19" t="s">
+      <c r="BF34" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL34" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
         <v>631</v>
       </c>
@@ -6662,27 +6720,24 @@
       <c r="U35" s="21"/>
       <c r="V35" s="21"/>
       <c r="W35" s="21"/>
-      <c r="AA35" s="21" t="s">
+      <c r="AV35" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB35" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI35">
+      <c r="AW35" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD35">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ35" s="21" t="s">
+      <c r="BE35" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK35" s="21" t="s">
+      <c r="BF35" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL35" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>631</v>
       </c>
@@ -6716,27 +6771,24 @@
       <c r="U36" s="19"/>
       <c r="V36" s="19"/>
       <c r="W36" s="19"/>
-      <c r="AA36" s="19" t="s">
+      <c r="AV36" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB36" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI36">
+      <c r="AW36" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD36">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ36" s="19" t="s">
+      <c r="BE36" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK36" s="19" t="s">
+      <c r="BF36" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL36" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>631</v>
       </c>
@@ -6770,27 +6822,24 @@
       <c r="U37" s="21"/>
       <c r="V37" s="21"/>
       <c r="W37" s="21"/>
-      <c r="AA37" s="21" t="s">
+      <c r="AV37" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="AB37" s="21">
+      <c r="AW37" s="21">
         <v>48</v>
       </c>
-      <c r="AI37">
+      <c r="BD37">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AJ37" s="21" t="s">
+      <c r="BE37" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="AK37" s="21" t="s">
+      <c r="BF37" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="AL37" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>631</v>
       </c>
@@ -6824,27 +6873,24 @@
       <c r="U38" s="19"/>
       <c r="V38" s="19"/>
       <c r="W38" s="19"/>
-      <c r="AA38" s="19" t="s">
+      <c r="AV38" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="AB38" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI38">
+      <c r="AW38" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD38">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ38" s="19" t="s">
+      <c r="BE38" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="AK38" s="19" t="s">
+      <c r="BF38" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="AL38" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
         <v>631</v>
       </c>
@@ -6878,27 +6924,24 @@
       <c r="U39" s="21"/>
       <c r="V39" s="21"/>
       <c r="W39" s="21"/>
-      <c r="AA39" s="21" t="s">
+      <c r="AV39" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AB39" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI39">
+      <c r="AW39" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD39">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ39" s="21" t="s">
+      <c r="BE39" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AK39" s="21" t="s">
+      <c r="BF39" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AL39" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>631</v>
       </c>
@@ -6932,27 +6975,24 @@
       <c r="U40" s="19"/>
       <c r="V40" s="19"/>
       <c r="W40" s="19"/>
-      <c r="AA40" s="19" t="s">
+      <c r="AV40" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB40" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI40">
+      <c r="AW40" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD40">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ40" s="19" t="s">
+      <c r="BE40" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK40" s="19" t="s">
+      <c r="BF40" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL40" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>631</v>
       </c>
@@ -6986,27 +7026,24 @@
       <c r="U41" s="21"/>
       <c r="V41" s="21"/>
       <c r="W41" s="21"/>
-      <c r="AA41" s="21" t="s">
+      <c r="AV41" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB41" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI41">
+      <c r="AW41" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD41">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ41" s="21" t="s">
+      <c r="BE41" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK41" s="21" t="s">
+      <c r="BF41" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL41" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>631</v>
       </c>
@@ -7040,27 +7077,24 @@
       <c r="U42" s="19"/>
       <c r="V42" s="19"/>
       <c r="W42" s="19"/>
-      <c r="AA42" s="19" t="s">
+      <c r="AV42" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB42" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI42">
+      <c r="AW42" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD42">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ42" s="19" t="s">
+      <c r="BE42" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK42" s="19" t="s">
+      <c r="BF42" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL42" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>631</v>
       </c>
@@ -7094,27 +7128,24 @@
       <c r="U43" s="21"/>
       <c r="V43" s="21"/>
       <c r="W43" s="21"/>
-      <c r="AA43" s="21" t="s">
+      <c r="AV43" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB43" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI43">
+      <c r="AW43" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD43">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ43" s="21" t="s">
+      <c r="BE43" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK43" s="21" t="s">
+      <c r="BF43" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL43" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>631</v>
       </c>
@@ -7148,27 +7179,24 @@
       <c r="U44" s="19"/>
       <c r="V44" s="19"/>
       <c r="W44" s="19"/>
-      <c r="AA44" s="19" t="s">
+      <c r="AV44" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB44" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI44">
+      <c r="AW44" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD44">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ44" s="19" t="s">
+      <c r="BE44" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK44" s="19" t="s">
+      <c r="BF44" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL44" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>631</v>
       </c>
@@ -7202,27 +7230,24 @@
       <c r="U45" s="21"/>
       <c r="V45" s="21"/>
       <c r="W45" s="21"/>
-      <c r="AA45" s="21" t="s">
+      <c r="AV45" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB45" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI45">
+      <c r="AW45" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD45">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ45" s="21" t="s">
+      <c r="BE45" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK45" s="21" t="s">
+      <c r="BF45" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL45" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>631</v>
       </c>
@@ -7256,27 +7281,24 @@
       <c r="U46" s="19"/>
       <c r="V46" s="19"/>
       <c r="W46" s="19"/>
-      <c r="AA46" s="19" t="s">
+      <c r="AV46" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB46" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI46">
+      <c r="AW46" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD46">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ46" s="19" t="s">
+      <c r="BE46" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK46" s="19" t="s">
+      <c r="BF46" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL46" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>631</v>
       </c>
@@ -7310,27 +7332,24 @@
       <c r="U47" s="21"/>
       <c r="V47" s="21"/>
       <c r="W47" s="21"/>
-      <c r="AA47" s="21" t="s">
+      <c r="AV47" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB47" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI47">
+      <c r="AW47" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD47">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ47" s="21" t="s">
+      <c r="BE47" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK47" s="21" t="s">
+      <c r="BF47" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL47" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>631</v>
       </c>
@@ -7364,27 +7383,24 @@
       <c r="U48" s="19"/>
       <c r="V48" s="19"/>
       <c r="W48" s="19"/>
-      <c r="AA48" s="19" t="s">
+      <c r="AV48" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB48" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI48">
+      <c r="AW48" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD48">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ48" s="19" t="s">
+      <c r="BE48" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK48" s="19" t="s">
+      <c r="BF48" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL48" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="49" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>631</v>
       </c>
@@ -7418,27 +7434,24 @@
       <c r="U49" s="21"/>
       <c r="V49" s="21"/>
       <c r="W49" s="21"/>
-      <c r="AA49" s="21" t="s">
+      <c r="AV49" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB49" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI49">
+      <c r="AW49" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD49">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ49" s="21" t="s">
+      <c r="BE49" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK49" s="21" t="s">
+      <c r="BF49" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL49" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="50" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
         <v>631</v>
       </c>
@@ -7472,27 +7485,24 @@
       <c r="U50" s="19"/>
       <c r="V50" s="19"/>
       <c r="W50" s="19"/>
-      <c r="AA50" s="19" t="s">
+      <c r="AV50" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="AB50" s="19">
+      <c r="AW50" s="19">
         <v>48</v>
       </c>
-      <c r="AI50">
+      <c r="BD50">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AJ50" s="19" t="s">
+      <c r="BE50" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="AK50" s="19" t="s">
+      <c r="BF50" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="AL50" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="51" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>631</v>
       </c>
@@ -7526,27 +7536,24 @@
       <c r="U51" s="21"/>
       <c r="V51" s="21"/>
       <c r="W51" s="21"/>
-      <c r="AA51" s="21" t="s">
+      <c r="AV51" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="AB51" s="21">
+      <c r="AW51" s="21">
         <v>48</v>
       </c>
-      <c r="AI51">
+      <c r="BD51">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AJ51" s="21" t="s">
+      <c r="BE51" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="AK51" s="21" t="s">
+      <c r="BF51" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="AL51" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="52" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
         <v>631</v>
       </c>
@@ -7580,27 +7587,24 @@
       <c r="U52" s="19"/>
       <c r="V52" s="19"/>
       <c r="W52" s="19"/>
-      <c r="AA52" s="19" t="s">
+      <c r="AV52" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB52" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI52">
+      <c r="AW52" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD52">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ52" s="19" t="s">
+      <c r="BE52" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK52" s="19" t="s">
+      <c r="BF52" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL52" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="53" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>631</v>
       </c>
@@ -7634,27 +7638,24 @@
       <c r="U53" s="21"/>
       <c r="V53" s="21"/>
       <c r="W53" s="21"/>
-      <c r="AA53" s="21" t="s">
+      <c r="AV53" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB53" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI53">
+      <c r="AW53" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD53">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ53" s="21" t="s">
+      <c r="BE53" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK53" s="21" t="s">
+      <c r="BF53" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL53" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="54" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
         <v>631</v>
       </c>
@@ -7688,27 +7689,24 @@
       <c r="U54" s="19"/>
       <c r="V54" s="19"/>
       <c r="W54" s="19"/>
-      <c r="AA54" s="19" t="s">
+      <c r="AV54" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB54" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI54">
+      <c r="AW54" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD54">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ54" s="19" t="s">
+      <c r="BE54" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK54" s="19" t="s">
+      <c r="BF54" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL54" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="55" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>631</v>
       </c>
@@ -7742,27 +7740,24 @@
       <c r="U55" s="21"/>
       <c r="V55" s="21"/>
       <c r="W55" s="21"/>
-      <c r="AA55" s="21" t="s">
+      <c r="AV55" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB55" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI55">
+      <c r="AW55" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD55">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ55" s="21" t="s">
+      <c r="BE55" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK55" s="21" t="s">
+      <c r="BF55" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL55" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="56" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>631</v>
       </c>
@@ -7796,27 +7791,24 @@
       <c r="U56" s="19"/>
       <c r="V56" s="19"/>
       <c r="W56" s="19"/>
-      <c r="AA56" s="19" t="s">
+      <c r="AV56" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB56" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI56">
+      <c r="AW56" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD56">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ56" s="19" t="s">
+      <c r="BE56" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK56" s="19" t="s">
+      <c r="BF56" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL56" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="57" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>631</v>
       </c>
@@ -7850,27 +7842,24 @@
       <c r="U57" s="21"/>
       <c r="V57" s="21"/>
       <c r="W57" s="21"/>
-      <c r="AA57" s="21" t="s">
+      <c r="AV57" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB57" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI57">
+      <c r="AW57" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD57">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ57" s="21" t="s">
+      <c r="BE57" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK57" s="21" t="s">
+      <c r="BF57" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL57" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="58" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
         <v>631</v>
       </c>
@@ -7904,27 +7893,24 @@
       <c r="U58" s="19"/>
       <c r="V58" s="19"/>
       <c r="W58" s="19"/>
-      <c r="AA58" s="19" t="s">
+      <c r="AV58" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB58" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI58">
+      <c r="AW58" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD58">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ58" s="19" t="s">
+      <c r="BE58" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK58" s="19" t="s">
+      <c r="BF58" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL58" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="59" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>631</v>
       </c>
@@ -7958,27 +7944,24 @@
       <c r="U59" s="21"/>
       <c r="V59" s="21"/>
       <c r="W59" s="21"/>
-      <c r="AA59" s="21" t="s">
+      <c r="AV59" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="AB59" s="21">
+      <c r="AW59" s="21">
         <v>48</v>
       </c>
-      <c r="AI59">
+      <c r="BD59">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AJ59" s="21" t="s">
+      <c r="BE59" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="AK59" s="21" t="s">
+      <c r="BF59" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="AL59" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="60" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
         <v>631</v>
       </c>
@@ -8012,27 +7995,24 @@
       <c r="U60" s="19"/>
       <c r="V60" s="19"/>
       <c r="W60" s="19"/>
-      <c r="AA60" s="19" t="s">
+      <c r="AV60" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB60" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI60">
+      <c r="AW60" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD60">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ60" s="19" t="s">
+      <c r="BE60" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK60" s="19" t="s">
+      <c r="BF60" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL60" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="61" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>631</v>
       </c>
@@ -8066,27 +8046,24 @@
       <c r="U61" s="21"/>
       <c r="V61" s="21"/>
       <c r="W61" s="21"/>
-      <c r="AA61" s="21" t="s">
+      <c r="AV61" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB61" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI61">
+      <c r="AW61" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD61">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ61" s="21" t="s">
+      <c r="BE61" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK61" s="21" t="s">
+      <c r="BF61" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL61" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="62" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
         <v>631</v>
       </c>
@@ -8120,27 +8097,24 @@
       <c r="U62" s="19"/>
       <c r="V62" s="19"/>
       <c r="W62" s="19"/>
-      <c r="AA62" s="19" t="s">
+      <c r="AV62" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB62" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI62">
+      <c r="AW62" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD62">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ62" s="19" t="s">
+      <c r="BE62" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK62" s="19" t="s">
+      <c r="BF62" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL62" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="63" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
         <v>631</v>
       </c>
@@ -8174,27 +8148,24 @@
       <c r="U63" s="21"/>
       <c r="V63" s="21"/>
       <c r="W63" s="21"/>
-      <c r="AA63" s="21" t="s">
+      <c r="AV63" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AB63" s="21">
+      <c r="AW63" s="21">
         <v>48</v>
       </c>
-      <c r="AI63">
+      <c r="BD63">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="AJ63" s="21" t="s">
+      <c r="BE63" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AK63" s="21" t="s">
+      <c r="BF63" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="AL63" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="64" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
         <v>631</v>
       </c>
@@ -8228,27 +8199,24 @@
       <c r="U64" s="19"/>
       <c r="V64" s="19"/>
       <c r="W64" s="19"/>
-      <c r="AA64" s="19" t="s">
+      <c r="AV64" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB64" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI64">
+      <c r="AW64" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD64">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ64" s="19" t="s">
+      <c r="BE64" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK64" s="19" t="s">
+      <c r="BF64" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL64" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="65" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>631</v>
       </c>
@@ -8282,27 +8250,24 @@
       <c r="U65" s="21"/>
       <c r="V65" s="21"/>
       <c r="W65" s="21"/>
-      <c r="AA65" s="21" t="s">
+      <c r="AV65" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB65" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI65">
+      <c r="AW65" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD65">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ65" s="21" t="s">
+      <c r="BE65" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK65" s="21" t="s">
+      <c r="BF65" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL65" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="66" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
         <v>631</v>
       </c>
@@ -8336,27 +8301,24 @@
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
       <c r="W66" s="19"/>
-      <c r="AA66" s="19" t="s">
+      <c r="AV66" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB66" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI66">
+      <c r="AW66" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD66">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ66" s="19" t="s">
+      <c r="BE66" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK66" s="19" t="s">
+      <c r="BF66" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL66" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="67" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>631</v>
       </c>
@@ -8390,27 +8352,24 @@
       <c r="U67" s="21"/>
       <c r="V67" s="21"/>
       <c r="W67" s="21"/>
-      <c r="AA67" s="21" t="s">
+      <c r="AV67" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB67" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI67">
-        <f t="shared" ref="AI67:AI78" si="1">SUM(AB67,AD67,AF67,AH67)</f>
-        <v>24</v>
-      </c>
-      <c r="AJ67" s="21" t="s">
+      <c r="AW67" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD67">
+        <f t="shared" ref="BD67:BD78" si="1">SUM(AW67,AY67,BA67,BC67)</f>
+        <v>24</v>
+      </c>
+      <c r="BE67" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK67" s="21" t="s">
+      <c r="BF67" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL67" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="68" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
         <v>631</v>
       </c>
@@ -8444,27 +8403,24 @@
       <c r="U68" s="19"/>
       <c r="V68" s="19"/>
       <c r="W68" s="19"/>
-      <c r="AA68" s="19" t="s">
+      <c r="AV68" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB68" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI68">
+      <c r="AW68" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD68">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ68" s="19" t="s">
+      <c r="BE68" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK68" s="19" t="s">
+      <c r="BF68" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL68" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="69" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>631</v>
       </c>
@@ -8498,27 +8454,24 @@
       <c r="U69" s="21"/>
       <c r="V69" s="21"/>
       <c r="W69" s="21"/>
-      <c r="AA69" s="21" t="s">
+      <c r="AV69" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB69" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI69">
+      <c r="AW69" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD69">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ69" s="21" t="s">
+      <c r="BE69" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK69" s="21" t="s">
+      <c r="BF69" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL69" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="70" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
         <v>631</v>
       </c>
@@ -8552,27 +8505,24 @@
       <c r="U70" s="19"/>
       <c r="V70" s="19"/>
       <c r="W70" s="19"/>
-      <c r="AA70" s="19" t="s">
+      <c r="AV70" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB70" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI70">
+      <c r="AW70" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD70">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ70" s="19" t="s">
+      <c r="BE70" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK70" s="19" t="s">
+      <c r="BF70" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL70" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="71" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>631</v>
       </c>
@@ -8606,27 +8556,24 @@
       <c r="U71" s="21"/>
       <c r="V71" s="21"/>
       <c r="W71" s="21"/>
-      <c r="AA71" s="21" t="s">
+      <c r="AV71" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB71" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI71">
+      <c r="AW71" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD71">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ71" s="21" t="s">
+      <c r="BE71" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK71" s="21" t="s">
+      <c r="BF71" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL71" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="72" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
         <v>631</v>
       </c>
@@ -8660,27 +8607,24 @@
       <c r="U72" s="19"/>
       <c r="V72" s="19"/>
       <c r="W72" s="19"/>
-      <c r="AA72" s="19" t="s">
+      <c r="AV72" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB72" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI72">
+      <c r="AW72" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD72">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ72" s="19" t="s">
+      <c r="BE72" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK72" s="19" t="s">
+      <c r="BF72" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL72" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="73" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>631</v>
       </c>
@@ -8714,27 +8658,24 @@
       <c r="U73" s="21"/>
       <c r="V73" s="21"/>
       <c r="W73" s="21"/>
-      <c r="AA73" s="21" t="s">
+      <c r="AV73" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB73" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI73">
+      <c r="AW73" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD73">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ73" s="21" t="s">
+      <c r="BE73" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK73" s="21" t="s">
+      <c r="BF73" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL73" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="74" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
         <v>631</v>
       </c>
@@ -8768,27 +8709,24 @@
       <c r="U74" s="19"/>
       <c r="V74" s="19"/>
       <c r="W74" s="19"/>
-      <c r="AA74" s="19" t="s">
+      <c r="AV74" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB74" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI74">
+      <c r="AW74" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD74">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ74" s="19" t="s">
+      <c r="BE74" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK74" s="19" t="s">
+      <c r="BF74" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL74" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="75" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>631</v>
       </c>
@@ -8822,27 +8760,24 @@
       <c r="U75" s="21"/>
       <c r="V75" s="21"/>
       <c r="W75" s="21"/>
-      <c r="AA75" s="21" t="s">
+      <c r="AV75" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB75" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI75">
+      <c r="AW75" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD75">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ75" s="21" t="s">
+      <c r="BE75" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK75" s="21" t="s">
+      <c r="BF75" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL75" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="76" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
         <v>631</v>
       </c>
@@ -8876,27 +8811,24 @@
       <c r="U76" s="19"/>
       <c r="V76" s="19"/>
       <c r="W76" s="19"/>
-      <c r="AA76" s="19" t="s">
+      <c r="AV76" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB76" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI76">
+      <c r="AW76" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD76">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ76" s="19" t="s">
+      <c r="BE76" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK76" s="19" t="s">
+      <c r="BF76" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL76" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="77" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>631</v>
       </c>
@@ -8930,27 +8862,24 @@
       <c r="U77" s="21"/>
       <c r="V77" s="21"/>
       <c r="W77" s="21"/>
-      <c r="AA77" s="21" t="s">
+      <c r="AV77" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB77" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI77">
+      <c r="AW77" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD77">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="AJ77" s="21" t="s">
+      <c r="BE77" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK77" s="21" t="s">
+      <c r="BF77" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL77" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="78" spans="1:38" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
         <v>631</v>
       </c>
@@ -8984,24 +8913,21 @@
       <c r="U78" s="19"/>
       <c r="V78" s="19"/>
       <c r="W78" s="19"/>
-      <c r="AA78" s="19" t="s">
+      <c r="AV78" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="AB78" s="19">
+      <c r="AW78" s="19">
         <v>48</v>
       </c>
-      <c r="AI78">
+      <c r="BD78">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="AJ78" s="19" t="s">
+      <c r="BE78" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="AK78" s="19" t="s">
+      <c r="BF78" s="19" t="s">
         <v>74</v>
-      </c>
-      <c r="AL78" t="s">
-        <v>888</v>
       </c>
     </row>
   </sheetData>
@@ -9013,10 +8939,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL7"/>
+  <dimension ref="A1:BG7"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AG7" sqref="AG7"/>
+    <sheetView topLeftCell="AT1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="BD9" sqref="BD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9046,7 +8972,7 @@
     <col min="24" max="24" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>15</v>
       </c>
@@ -9117,52 +9043,115 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>955</v>
+        <v>878</v>
       </c>
       <c r="Y1" t="s">
-        <v>956</v>
+        <v>879</v>
       </c>
       <c r="Z1" t="s">
         <v>22</v>
       </c>
       <c r="AA1" t="s">
+        <v>890</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>891</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>892</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>893</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>894</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>895</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>896</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>897</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>879</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AW1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="36" t="s">
-        <v>957</v>
-      </c>
-      <c r="AD1" s="36" t="s">
-        <v>958</v>
-      </c>
-      <c r="AE1" s="36" t="s">
-        <v>959</v>
-      </c>
-      <c r="AF1" s="36" t="s">
-        <v>960</v>
-      </c>
-      <c r="AG1" s="36" t="s">
-        <v>961</v>
-      </c>
-      <c r="AH1" s="36" t="s">
-        <v>962</v>
-      </c>
-      <c r="AI1" s="37" t="s">
-        <v>963</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AX1" s="36" t="s">
+        <v>880</v>
+      </c>
+      <c r="AY1" s="36" t="s">
+        <v>881</v>
+      </c>
+      <c r="AZ1" s="36" t="s">
+        <v>882</v>
+      </c>
+      <c r="BA1" s="36" t="s">
+        <v>883</v>
+      </c>
+      <c r="BB1" s="36" t="s">
+        <v>884</v>
+      </c>
+      <c r="BC1" s="36" t="s">
+        <v>885</v>
+      </c>
+      <c r="BD1" s="37" t="s">
+        <v>886</v>
+      </c>
+      <c r="BE1" t="s">
         <v>42</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="BF1" t="s">
         <v>43</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="BG1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>130</v>
       </c>
@@ -9226,27 +9215,27 @@
       <c r="U2" s="19"/>
       <c r="V2" s="19"/>
       <c r="W2" s="19"/>
-      <c r="AA2" s="19" t="s">
+      <c r="AV2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI2">
-        <f>SUM(AB2,AD2,AF2,AH2)</f>
-        <v>24</v>
-      </c>
-      <c r="AJ2" s="19" t="s">
+      <c r="AW2" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD2">
+        <f>SUM(AW2,AY2,BA2,BC2)</f>
+        <v>24</v>
+      </c>
+      <c r="BE2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK2" s="19" t="s">
+      <c r="BF2" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL2" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG2" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>130</v>
       </c>
@@ -9280,27 +9269,27 @@
       <c r="U3" s="21"/>
       <c r="V3" s="21"/>
       <c r="W3" s="21"/>
-      <c r="AA3" s="21" t="s">
+      <c r="AV3" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB3" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI3">
-        <f t="shared" ref="AI3:AI7" si="0">SUM(AB3,AD3,AF3,AH3)</f>
-        <v>24</v>
-      </c>
-      <c r="AJ3" s="21" t="s">
+      <c r="AW3" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD3">
+        <f t="shared" ref="BD3:BD7" si="0">SUM(AW3,AY3,BA3,BC3)</f>
+        <v>24</v>
+      </c>
+      <c r="BE3" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK3" s="21" t="s">
+      <c r="BF3" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL3" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG3" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>130</v>
       </c>
@@ -9370,27 +9359,27 @@
       <c r="W4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AA4" s="19" t="s">
+      <c r="AV4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB4" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI4">
+      <c r="AW4" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD4">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ4" s="19" t="s">
+      <c r="BE4" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK4" s="19" t="s">
+      <c r="BF4" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL4" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG4" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>130</v>
       </c>
@@ -9424,27 +9413,27 @@
       <c r="U5" s="21"/>
       <c r="V5" s="21"/>
       <c r="W5" s="21"/>
-      <c r="AA5" s="21" t="s">
+      <c r="AV5" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB5" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI5">
+      <c r="AW5" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD5">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ5" s="21" t="s">
+      <c r="BE5" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK5" s="21" t="s">
+      <c r="BF5" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL5" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG5" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>130</v>
       </c>
@@ -9508,27 +9497,27 @@
       <c r="U6" s="22"/>
       <c r="V6" s="22"/>
       <c r="W6" s="19"/>
-      <c r="AA6" s="19" t="s">
+      <c r="AV6" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="AB6" s="19">
-        <v>24</v>
-      </c>
-      <c r="AI6">
+      <c r="AW6" s="19">
+        <v>24</v>
+      </c>
+      <c r="BD6">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ6" s="19" t="s">
+      <c r="BE6" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AK6" s="19" t="s">
+      <c r="BF6" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="AL6" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="BG6" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>130</v>
       </c>
@@ -9598,24 +9587,24 @@
       <c r="W7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="AA7" s="21" t="s">
+      <c r="AV7" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="AB7" s="21">
-        <v>24</v>
-      </c>
-      <c r="AI7">
+      <c r="AW7" s="21">
+        <v>24</v>
+      </c>
+      <c r="BD7">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ7" s="21" t="s">
+      <c r="BE7" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="AK7" s="21" t="s">
+      <c r="BF7" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="AL7" t="s">
-        <v>896</v>
+      <c r="BG7" t="s">
+        <v>819</v>
       </c>
     </row>
   </sheetData>
@@ -9629,7 +9618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
@@ -12210,7 +12199,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>